<commit_message>
updated how we calculate total kelp cover
</commit_message>
<xml_diff>
--- a/metadata/Kelp cover photograph 2019 GPS locations.xlsx
+++ b/metadata/Kelp cover photograph 2019 GPS locations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A22171\Dropbox\ArcticKelp Canada\ArcticKelp Canada Shared\Master files\raw data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A22171\Dropbox\ArcticKelp Canada\ArcticKelp Canada Shared\ArcticKelp\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE671583-55EC-4D7A-81DF-4F60307CAEE5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E5F6E1-207B-488B-8CF8-E2153865697B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43485" yWindow="810" windowWidth="13770" windowHeight="13755" xr2:uid="{4958167B-6B3B-4E55-A6B1-B1A00EB6174D}"/>
+    <workbookView xWindow="32850" yWindow="465" windowWidth="18705" windowHeight="13545" xr2:uid="{4958167B-6B3B-4E55-A6B1-B1A00EB6174D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="43">
   <si>
     <t>Campaign</t>
   </si>
@@ -151,6 +151,15 @@
   </si>
   <si>
     <t>Mussel Point</t>
+  </si>
+  <si>
+    <t>Pangnirtung NFA</t>
+  </si>
+  <si>
+    <t>Pangnirtung 1</t>
+  </si>
+  <si>
+    <t>Pangnirtung 2</t>
   </si>
 </sst>
 </file>
@@ -523,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D64C6AAB-DE6E-45F3-8ED9-5DEFDAB1D6AC}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1047,7 +1056,7 @@
         <v>-64.340999999999994</v>
       </c>
       <c r="F25" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -1147,6 +1156,50 @@
         <v>-59.195999999999998</v>
       </c>
       <c r="F30" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="1">
+        <v>43746</v>
+      </c>
+      <c r="C31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31">
+        <f>66+(6.4/60)</f>
+        <v>66.106666666666669</v>
+      </c>
+      <c r="E31">
+        <f>-59.5/60-65</f>
+        <v>-65.99166666666666</v>
+      </c>
+      <c r="F31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32" s="1">
+        <v>43746</v>
+      </c>
+      <c r="C32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32">
+        <f>66+(15.96/60)</f>
+        <v>66.266000000000005</v>
+      </c>
+      <c r="E32">
+        <f>-59.5/60-67</f>
+        <v>-67.99166666666666</v>
+      </c>
+      <c r="F32" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2 more sites in
</commit_message>
<xml_diff>
--- a/metadata/Kelp cover photograph 2019 GPS locations.xlsx
+++ b/metadata/Kelp cover photograph 2019 GPS locations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A22171\Dropbox\ArcticKelp Canada\ArcticKelp Canada Shared\ArcticKelp\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C4979E-4705-45B5-B01C-C931D8E90E95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FB1ADB-8048-4573-B3D1-F1CF1E540CF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1480" windowWidth="14400" windowHeight="9320" xr2:uid="{4958167B-6B3B-4E55-A6B1-B1A00EB6174D}"/>
+    <workbookView xWindow="29355" yWindow="600" windowWidth="23325" windowHeight="14475" xr2:uid="{4958167B-6B3B-4E55-A6B1-B1A00EB6174D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -535,7 +535,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1076,7 +1076,7 @@
         <v>-63.73</v>
       </c>
       <c r="F26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
@@ -1096,7 +1096,7 @@
         <v>-63.523000000000003</v>
       </c>
       <c r="F27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
@@ -1116,7 +1116,7 @@
         <v>-61.307000000000002</v>
       </c>
       <c r="F28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
@@ -1136,7 +1136,7 @@
         <v>-59.174999999999997</v>
       </c>
       <c r="F29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
@@ -1156,7 +1156,7 @@
         <v>-59.195999999999998</v>
       </c>
       <c r="F30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
so much data new data! Am on an image analysis roll.  I've also added the GPS points and double checked them
</commit_message>
<xml_diff>
--- a/metadata/Kelp cover photograph 2019 GPS locations.xlsx
+++ b/metadata/Kelp cover photograph 2019 GPS locations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\A22171\Dropbox\ArcticKelp Canada\ArcticKelp Canada Shared\ArcticKelp\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FB1ADB-8048-4573-B3D1-F1CF1E540CF1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6180F476-4F2C-40A6-99D8-BF9F1461804E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29355" yWindow="600" windowWidth="23325" windowHeight="14475" xr2:uid="{4958167B-6B3B-4E55-A6B1-B1A00EB6174D}"/>
+    <workbookView xWindow="620" yWindow="810" windowWidth="18580" windowHeight="9990" xr2:uid="{4958167B-6B3B-4E55-A6B1-B1A00EB6174D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="50">
   <si>
     <t>Campaign</t>
   </si>
@@ -138,28 +138,49 @@
     <t>entered</t>
   </si>
   <si>
+    <t>Evan's Bight</t>
+  </si>
+  <si>
+    <t>Turnagain</t>
+  </si>
+  <si>
+    <t>Makkovik</t>
+  </si>
+  <si>
+    <t>Mussel Point</t>
+  </si>
+  <si>
+    <t>Pangnirtung NFA</t>
+  </si>
+  <si>
+    <t>Pangnirtung 1</t>
+  </si>
+  <si>
+    <t>Pangnirtung 2</t>
+  </si>
+  <si>
+    <t>CAISN DFO</t>
+  </si>
+  <si>
     <t>not entered</t>
   </si>
   <si>
-    <t>Evan's Bight</t>
-  </si>
-  <si>
-    <t>Turnagain</t>
-  </si>
-  <si>
-    <t>Makkovik</t>
-  </si>
-  <si>
-    <t>Mussel Point</t>
-  </si>
-  <si>
-    <t>Pangnirtung NFA</t>
-  </si>
-  <si>
-    <t>Pangnirtung 1</t>
-  </si>
-  <si>
-    <t>Pangnirtung 2</t>
+    <t>Steensby Inlet T1</t>
+  </si>
+  <si>
+    <t>Deception Bay 4</t>
+  </si>
+  <si>
+    <t>Steensby Inlet T2</t>
+  </si>
+  <si>
+    <t>Steensby Inlet T3</t>
+  </si>
+  <si>
+    <t>Steensby Inlet T5</t>
+  </si>
+  <si>
+    <t>Steensby Inlet T6</t>
   </si>
 </sst>
 </file>
@@ -169,10 +190,29 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -213,11 +253,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D64C6AAB-DE6E-45F3-8ED9-5DEFDAB1D6AC}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1087,7 +1135,7 @@
         <v>41710</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D27" s="2">
         <v>59.298499999999997</v>
@@ -1107,7 +1155,7 @@
         <v>41711</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D28" s="2">
         <v>56.765999999999998</v>
@@ -1127,7 +1175,7 @@
         <v>41712</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D29" s="2">
         <v>55.088000000000001</v>
@@ -1147,7 +1195,7 @@
         <v>41713</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D30" s="2">
         <v>55.101999999999997</v>
@@ -1161,13 +1209,13 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="1">
         <v>43746</v>
       </c>
       <c r="C31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D31">
         <f>66+(6.4/60)</f>
@@ -1183,13 +1231,13 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B32" s="1">
         <v>43746</v>
       </c>
       <c r="C32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D32">
         <f>66+(15.96/60)</f>
@@ -1200,10 +1248,132 @@
         <v>-67.99166666666666</v>
       </c>
       <c r="F32" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A33" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="6">
+        <v>41122</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D33" s="7">
+        <v>62.245669999999997</v>
+      </c>
+      <c r="E33" s="7">
+        <v>-74.860870000000006</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="6">
+        <v>41136</v>
+      </c>
+      <c r="C34" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D34" s="7">
+        <v>62.245669999999997</v>
+      </c>
+      <c r="E34" s="7">
+        <v>-74.860870000000006</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="6">
+        <v>41140</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="4">
+        <v>70.214389999999995</v>
+      </c>
+      <c r="E35" s="4">
+        <v>-78.763810000000007</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B36" s="6">
+        <v>41138</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D36" s="4">
+        <v>70.196529999999996</v>
+      </c>
+      <c r="E36" s="4">
+        <v>-78.390879999999996</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B37" s="6">
+        <v>41139</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D37" s="4">
+        <v>70.273330000000001</v>
+      </c>
+      <c r="E37" s="4">
+        <v>-78.510069999999999</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="6">
+        <v>41139</v>
+      </c>
+      <c r="C38" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" s="4">
+        <v>70.32535</v>
+      </c>
+      <c r="E38" s="4">
+        <v>-78.562889999999996</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>